<commit_message>
update with 2021 stf
</commit_message>
<xml_diff>
--- a/NSAS/data/Catch/multi_fleet_HAWG2020.xlsx
+++ b/NSAS/data/Catch/multi_fleet_HAWG2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\wg_HAWG\NSAS\data\Catch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\git\wg_HAWG\NSAS\data\Catch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D52F80F7-4F85-4718-AA7C-205851A17AC9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12085313-CEDC-4CDA-98E4-2E8988933447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14355" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="2070" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -166,12 +176,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -241,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,13 +341,14 @@
     <xf numFmtId="171" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,10 +758,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:P70"/>
+  <dimension ref="A2:R70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -763,7 +780,7 @@
     <col min="16" max="16" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2019</v>
       </c>
@@ -792,7 +809,7 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -821,7 +838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -871,7 +888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
         <v>0</v>
       </c>
@@ -927,8 +944,12 @@
         <f>O5*N5</f>
         <v>3.5918953719394673</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R5" s="54">
+        <f>SUM(G5:G14)</f>
+        <v>5.1609999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>1</v>
       </c>
@@ -985,7 +1006,7 @@
         <v>6.3843346605473483</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>2</v>
       </c>
@@ -1042,7 +1063,7 @@
         <v>13.939423268387076</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
         <v>3</v>
       </c>
@@ -1099,7 +1120,7 @@
         <v>44.20710471780707</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
         <v>4</v>
       </c>
@@ -1156,7 +1177,7 @@
         <v>33.585829321861539</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>5</v>
       </c>
@@ -1213,7 +1234,7 @@
         <v>151.54130840058585</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <v>6</v>
       </c>
@@ -1270,7 +1291,7 @@
         <v>113.17443055947278</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>7</v>
       </c>
@@ -1327,7 +1348,7 @@
         <v>30.669384344091693</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
         <v>8</v>
       </c>
@@ -1384,7 +1405,7 @@
         <v>20.19404811651631</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>9</v>
       </c>
@@ -1441,7 +1462,7 @@
         <v>34.430750874551492</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>3</v>
       </c>
@@ -1475,39 +1496,39 @@
       </c>
       <c r="O15" s="23"/>
     </row>
-    <row r="16" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="51">
+      <c r="B16" s="52">
         <f>SUMPRODUCT(B5:B14,C5:C14)</f>
         <v>440.47099999999989</v>
       </c>
-      <c r="C16" s="51"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="26"/>
-      <c r="E16" s="52">
+      <c r="E16" s="53">
         <f>SUMPRODUCT(E5:E14,F5:F14)</f>
         <v>5.1609999999999996</v>
       </c>
-      <c r="F16" s="52"/>
+      <c r="F16" s="53"/>
       <c r="G16" s="27"/>
-      <c r="H16" s="52">
+      <c r="H16" s="53">
         <f>SUMPRODUCT(H5:H14,I5:I14)</f>
         <v>5.7697713211039137</v>
       </c>
-      <c r="I16" s="52"/>
+      <c r="I16" s="53"/>
       <c r="J16" s="27"/>
-      <c r="K16" s="52">
+      <c r="K16" s="53">
         <f>SUMPRODUCT(K5:K14,L5:L14)</f>
         <v>0.31673831465679736</v>
       </c>
-      <c r="L16" s="52"/>
+      <c r="L16" s="53"/>
       <c r="M16" s="27"/>
-      <c r="N16" s="52">
+      <c r="N16" s="53">
         <f>SUMPRODUCT(N5:N14,O5:O14)</f>
         <v>451.7185096357606</v>
       </c>
-      <c r="O16" s="52"/>
+      <c r="O16" s="53"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O17" s="11" t="s">
@@ -1653,7 +1674,7 @@
       <c r="H24" s="10">
         <v>13190</v>
       </c>
-      <c r="I24" s="53">
+      <c r="I24" s="51">
         <f>SUM(G5:G14)*1000</f>
         <v>5161</v>
       </c>

</xml_diff>